<commit_message>
Don't strip two first rows of the sheet.
</commit_message>
<xml_diff>
--- a/tests/fixtures/abcd.xlsx
+++ b/tests/fixtures/abcd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="D" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_GoBack" vbProcedure="false">B!$C$403</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_GoBack" vbProcedure="false">B!$C$401</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <r>
       <rPr>
@@ -60,9 +57,6 @@
     <t xml:space="preserve">(índice funcional) a, (direccional) ta </t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
     <t xml:space="preserve">baba</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">baba </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
   </si>
   <si>
     <r>
@@ -101,9 +92,6 @@
     <t xml:space="preserve">abrío, baje (s. m.)</t>
   </si>
   <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
     <t xml:space="preserve">dadivoso/a </t>
   </si>
   <si>
@@ -120,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -145,22 +133,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -209,20 +182,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,11 +195,7 @@
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,14 +205,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -273,8 +226,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -288,28 +241,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="876" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -519,7 +464,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -539,22 +484,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -580,7 +522,7 @@
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.29"/>
@@ -588,24 +530,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="5"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -625,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -644,27 +581,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>